<commit_message>
corrected gerbers for FM
</commit_message>
<xml_diff>
--- a/backplane/backplane-revC-foras-promineo-FM/bom/backplane_bom.xlsx
+++ b/backplane/backplane-revC-foras-promineo-FM/bom/backplane_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Item</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
     <t>SK68XX-EC3210R</t>
   </si>
   <si>
@@ -148,6 +142,54 @@
   </si>
   <si>
     <t>0mR</t>
+  </si>
+  <si>
+    <t>0.1uF 0402</t>
+  </si>
+  <si>
+    <t>1uF 0603</t>
+  </si>
+  <si>
+    <t>RGB LED 3210</t>
+  </si>
+  <si>
+    <t>Conn 4 pos</t>
+  </si>
+  <si>
+    <t>Conn 6 pos</t>
+  </si>
+  <si>
+    <t>Card Edge Connector, 120</t>
+  </si>
+  <si>
+    <t>Header 30x2</t>
+  </si>
+  <si>
+    <t>PNP SOT323</t>
+  </si>
+  <si>
+    <t>SMT SW</t>
+  </si>
+  <si>
+    <t>Mfr</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+  </si>
+  <si>
+    <t>YAEGO</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
   </si>
 </sst>
 </file>
@@ -971,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +1024,11 @@
     <col min="3" max="3" width="55.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -999,13 +1042,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1013,16 +1059,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1031,16 +1080,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>3</v>
@@ -1049,16 +1101,22 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1067,13 +1125,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1082,14 +1146,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1098,13 +1167,19 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1113,13 +1188,19 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1128,13 +1209,19 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1143,19 +1230,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1164,16 +1254,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1182,16 +1275,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1200,16 +1296,19 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1218,16 +1317,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1236,10 +1338,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>